<commit_message>
Flexi loan Sanity scenario
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4903-DISB-REPAYMENT-EXACTDATE-MoreAmt.xlsx
+++ b/Mifos Automation Excels/Client/4903-DISB-REPAYMENT-EXACTDATE-MoreAmt.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>clickonmakerepayment</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>$ 5,000</t>
-  </si>
-  <si>
-    <t>$ 9.61</t>
   </si>
   <si>
     <t>L88</t>
@@ -644,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
@@ -1657,7 +1654,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1802,7 @@
         <v>42036</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>42</v>
@@ -1816,8 +1813,8 @@
       <c r="G2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>54</v>
+      <c r="I2" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1831,7 +1828,7 @@
         <v>42036</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>42</v>
@@ -1843,7 +1840,7 @@
         <v>44</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1857,7 +1854,7 @@
         <v>42036</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>42</v>
@@ -1869,7 +1866,7 @@
         <v>45</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1881,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,7 +1939,7 @@
         <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1968,7 +1965,7 @@
         <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2003,7 +2000,7 @@
         <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2029,7 +2026,7 @@
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2064,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2090,7 +2087,7 @@
         <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>